<commit_message>
Added feedback for saved explanation Added feedback for file update Refactored code snippets and dir structure
</commit_message>
<xml_diff>
--- a/input-files/Ciscoccna.xlsx
+++ b/input-files/Ciscoccna.xlsx
@@ -1484,7 +1484,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Provide a simple, comprehensive, but concise rationale for the correct answer.</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>02fea6</t>
         </is>
       </c>
     </row>

</xml_diff>